<commit_message>
Final Updates + Company names
</commit_message>
<xml_diff>
--- a/app/src/data/resultat.xlsx
+++ b/app/src/data/resultat.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,12 +461,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>71.74.12.34</t>
+          <t>e837f252af30cc222a1bce815e609a7354e1f9c814baefbb5d45e32a10563759</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '71.74.12.34' combination.</t>
+          <t>severity: The 'severity' field must contain a valid severity. Allowed values: [informational low medium high critical].</t>
         </is>
       </c>
     </row>
@@ -486,12 +486,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E8676686A42D6D5EB7957439297E288BFE5188B6</t>
+          <t>959a7df5c465fcd963a641d87c18a565</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: '959a7df5c465fcd963a641d87c18a565' combination.</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>109.12.111.14</t>
+          <t>91.206.14.151</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '109.12.111.14' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '91.206.14.151' combination.</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3D78C842B16AC7EAF3D9A092F4BDA00ABF3378E5</t>
+          <t>bbed408b87701b0132e26570fb9fa94cb4bd9ab7</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>189.210.115.207</t>
+          <t>5c0a549ae45d9abe54ab662e53c484e2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '189.210.115.207' combination.</t>
+          <t>severity: The 'severity' field must contain a valid severity. Allowed values: [informational low medium high critical].</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4ED7609CBB86EA0B7607B8A002E7F85B316903C3B6801240C9576AAE8B3052FF</t>
+          <t>1df11bc19aa52b623bdf15380e3fded56d8eb6fb7b53a2240779864b1a6474ad</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '4ed7609cbb86ea0b7607b8a002e7f85b316903c3b6801240c9576aae8b3052ff' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '1df11bc19aa52b623bdf15380e3fded56d8eb6fb7b53a2240779864b1a6474ad' combination.</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14E7CC2EADC7C9BAC1930F37E25303212C8974674B21ED052A483727836A5E43</t>
+          <t>2d2030dee51b98bdeb397cfb93f897a5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '14e7cc2eadc7c9bac1930f37e25303212c8974674b21ed052a483727836a5e43' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '2d2030dee51b98bdeb397cfb93f897a5' combination.</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>F7205F07677F0A0995CB232E3CBC7F73</t>
+          <t>632f1c77337cca803467f7d368233cc59e9f0c6a</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'f7205f07677f0a0995cb232e3cbc7f73' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2897721785645AD5B2A8FB524ED650C0</t>
+          <t>5de37c17703e9b8d76222a30f2b1da22</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '2897721785645ad5b2a8fb524ed650c0' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '5de37c17703e9b8d76222a30f2b1da22' combination.</t>
         </is>
       </c>
     </row>
@@ -686,12 +686,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>75.188.35.168</t>
+          <t>31d223c813a592422461f0d6707ba571</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '75.188.35.168' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '31d223c813a592422461f0d6707ba571' combination.</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>ipv4</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>E9FF9B7E144BDAD9D8955F4A328F7B6DAA2B455E</t>
+          <t>213.226.71.125</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '213.226.71.125' combination.</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CFDF141404D8783F2C6181D185B3E1AD107E4169</t>
+          <t>43f46a66c821e143d77f9311b24314b5c5eeccfedbb3fbf1cd484c9e4f537a5d</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '43f46a66c821e143d77f9311b24314b5c5eeccfedbb3fbf1cd484c9e4f537a5d' combination.</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BAACFE8643EC95C12277961DABB411F2</t>
+          <t>040a4985172c82474459b384fe9269922ac0b98e</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'baacfe8643ec95c12277961dabb411f2' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>B595A580FDFE1308B47CF07805C81C32</t>
+          <t>https://crmweb.info:443/bitrix/rc9XjtwF/</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'b595a580fdfe1308b47cf07805c81c32' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>ipv4</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>BDF78C3E348A197847919EB1EDDA12E080072FAA</t>
+          <t>185.112.83.96</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '185.112.83.96' combination.</t>
         </is>
       </c>
     </row>
@@ -836,12 +836,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>54a77b0fc778a24e4214ad725734328e</t>
+          <t>http://accessunited-bank.com/admin/hzIgVwq8btak/</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '54a77b0fc778a24e4214ad725734328e' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3468b31f47a557fa45e096b6a212501f</t>
+          <t>d63a7756bfdcd2be6c755bf288a92c8b</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '3468b31f47a557fa45e096b6a212501f' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'd63a7756bfdcd2be6c755bf288a92c8b' combination.</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Domain</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>privacytoolzforyou6000.top</t>
+          <t>54270176a3484672055a816d13df613b5b614e0c</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'domain' and value: 'privacytoolzforyou6000.top' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -911,12 +911,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1535ea76379a3adb0a99d90f49af3801</t>
+          <t>http://pigij.com/wp-admin/MVW5/</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '1535ea76379a3adb0a99d90f49af3801' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>9F6E3B0B18F994950B40076D1386B4DA4CE0F1F973B129B32B363AAC4A678631</t>
+          <t>95e2fa71574c0cecbe15cf8fb4877bd97ce30ed0</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '9f6e3b0b18f994950b40076d1386b4da4ce0f1f973b129b32b363aac4a678631' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>82.77.137.101</t>
+          <t>0527026e0dc249e11533213908e979ab</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '82.77.137.101' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '0527026e0dc249e11533213908e979ab' combination.</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>76.25.142.196</t>
+          <t>ebb4c466a74b28546c04a94a28df781c80ad9c75</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '76.25.142.196' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>73.151.236.31</t>
+          <t>1785f4058c78ae3dd030808212ae3b04</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '73.151.236.31' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '1785f4058c78ae3dd030808212ae3b04' combination.</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CBFC135BFF84D63C4A0CCB5102CFA17D8C9BF297079F3B2F1371DAFCBEFEA77C</t>
+          <t>96d9b8d6658149ca78b2dc13e3f63bcd2dd87667</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'cbfc135bff84d63c4a0ccb5102cfa17d8c9bf297079f3b2f1371dafcbefea77c' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2615BD2173DAC44A6AD14702F3C93E67</t>
+          <t>b8293f2296ac09663e27759a39431fd6</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '2615bd2173dac44a6ad14702f3c93e67' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'b8293f2296ac09663e27759a39431fd6' combination.</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>956ECB4AFA437EAFE56F958B34B6A78303AD626BAEE004715DC6634B7546BF85</t>
+          <t>f3574a47570cccebb1c502287e21218277ffc589</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '956ecb4afa437eafe56f958b34b6a78303ad626baee004715dc6634b7546bf85' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>6C526A28ED49B2EF83548E20A71610877E69D450</t>
+          <t>d4aa276a7fbe8dcd858174eeacbb26ce</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'd4aa276a7fbe8dcd858174eeacbb26ce' combination.</t>
         </is>
       </c>
     </row>
@@ -1136,12 +1136,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>C789BB45CACF0DE1720E707F9EDD73B4ED0EDC958B3CE2D8F0AD5D4A7596923A</t>
+          <t>d9e94f076d175ace80f211ea298fa46e</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'c789bb45cacf0de1720e707f9edd73b4ed0edc958b3ce2d8f0ad5d4a7596923a' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'd9e94f076d175ace80f211ea298fa46e' combination.</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>92.59.35.196</t>
+          <t>ddf039c3d6395139fd7f31b0a796a444f385c582ca978779aae7314b19940812</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '92.59.35.196' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: 'ddf039c3d6395139fd7f31b0a796a444f385c582ca978779aae7314b19940812' combination.</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>24.55.112.61</t>
+          <t>7139415fecd716bec6d38d2004176f5d</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '24.55.112.61' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '7139415fecd716bec6d38d2004176f5d' combination.</t>
         </is>
       </c>
     </row>
@@ -1211,12 +1211,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>68.186.192.69</t>
+          <t>ef3e0845b289f1d3b5b234b0507c554dfdd23a5b77f36d433489129ea722c6bb</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '68.186.192.69' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: 'ef3e0845b289f1d3b5b234b0507c554dfdd23a5b77f36d433489129ea722c6bb' combination.</t>
         </is>
       </c>
     </row>
@@ -1236,12 +1236,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2F4085CB6A0B2DD4422F59894DCA5CF881EB8CCF</t>
+          <t>31f818372fa07d1fd158c91510b6a077</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: '31f818372fa07d1fd158c91510b6a077' combination.</t>
         </is>
       </c>
     </row>
@@ -1261,12 +1261,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2b8080284c0611ec7288a6d3e34a545f</t>
+          <t>http://strawberry.kids-singer.net/assets_c/WAdvNT84Dmu/</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '2b8080284c0611ec7288a6d3e34a545f' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1286,12 +1286,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>46.105.81.76</t>
+          <t>5f40e1859053b70df9c0753d327f2cee</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '46.105.81.76' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '5f40e1859053b70df9c0753d327f2cee' combination.</t>
         </is>
       </c>
     </row>
@@ -1311,12 +1311,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>a679d50a9d3a7d63704e33177f59bab9e4357be02ca916beab97f8b9daca29d8</t>
+          <t>https://eleccom.shop:443/services/AEjSDj/</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'a679d50a9d3a7d63704e33177f59bab9e4357be02ca916beab97f8b9daca29d8' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1336,12 +1336,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>06BE4CE3AEAE146A062B983CE21DD42B08CBA908A69958729E758BC41836735C</t>
+          <t>4ce0bdd2d4303bf77611b8b34c7d2883</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '06be4ce3aeae146a062b983ce21dd42b08cba908a69958729e758bc41836735c' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '4ce0bdd2d4303bf77611b8b34c7d2883' combination.</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3D913A4BA5C4F7810EC6B418D7A07B6207B60E740DDE8AED3E2DF9DDF1CAAB27</t>
+          <t>54d36e5dce2e546070dc0571c8b3e166d6df62296fa0609a325ace23b7105335</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '3d913a4ba5c4f7810ec6b418d7a07b6207b60e740dde8aed3e2df9ddf1caab27' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '54d36e5dce2e546070dc0571c8b3e166d6df62296fa0609a325ace23b7105335' combination.</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>185.7.214.7</t>
+          <t>8c4294e3154675cd926ab6b772dbbe0e7a49cae16f4a37d908e1ca6748251c43</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '185.7.214.7' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '8c4294e3154675cd926ab6b772dbbe0e7a49cae16f4a37d908e1ca6748251c43' combination.</t>
         </is>
       </c>
     </row>
@@ -1411,12 +1411,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>e4fbc46e6bf2830db3bbeac7ac96fe97b4ba8444</t>
+          <t>https://izocab.com/nashi-klienty/B5SC/</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1436,12 +1436,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CA564C6702D5E653ED8421349F4D37795D944793A3DBD1BB3C5DBC5732F1B798</t>
+          <t>58e8043876f2f302fbc98d00c270778b</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'ca564c6702d5e653ed8421349f4d37795d944793a3dbd1bb3c5dbc5732f1b798' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '58e8043876f2f302fbc98d00c270778b' combination.</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>de3dc22cc6f9cfd7670517be6ad18f78f79e6248c32d2ff5af91224e837c9bd3</t>
+          <t>526215dda9d0e85bcb6bce827f3f85d2</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'de3dc22cc6f9cfd7670517be6ad18f78f79e6248c32d2ff5af91224e837c9bd3' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '526215dda9d0e85bcb6bce827f3f85d2' combination.</t>
         </is>
       </c>
     </row>
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>EEE7C801BE1C21FA4791BBE9958EE68C66165B53</t>
+          <t>38cd6b79c832b575aa04221e608cbb7e</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>severity: The 'severity' field must contain a valid severity. Allowed values: [informational low medium high critical].</t>
         </is>
       </c>
     </row>
@@ -1511,12 +1511,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>27.223.92.142</t>
+          <t>e479a80de91ef78dbbf7f46363e59828</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '27.223.92.142' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'e479a80de91ef78dbbf7f46363e59828' combination.</t>
         </is>
       </c>
     </row>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>f82332b945a2ed02ad8edd45c90e0a7d8ba2193f</t>
+          <t>cea6be26d81a8ff3db0d9da666cd0f8f</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'cea6be26d81a8ff3db0d9da666cd0f8f' combination.</t>
         </is>
       </c>
     </row>
@@ -1561,12 +1561,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2.56.59.42</t>
+          <t>0c7b8da133799dd72d0dbe3ea012031e</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '2.56.59.42' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '0c7b8da133799dd72d0dbe3ea012031e' combination.</t>
         </is>
       </c>
     </row>
@@ -1586,12 +1586,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>eb00f5ad5cdb3e202378f32c5e135f2a</t>
+          <t>3d1fb09a9a05ab6cf83c4e7cdf5fe40e67064063</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'eb00f5ad5cdb3e202378f32c5e135f2a' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1611,12 +1611,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>FCC49C9BE5591F241FFD98DB0752CB9E20A97E881969537FBA5C513ADBD72814</t>
+          <t>28b791746c97c0c04dcbfe0954e7173b</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'fcc49c9be5591f241ffd98db0752cb9e20a97e881969537fba5c513adbd72814' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '28b791746c97c0c04dcbfe0954e7173b' combination.</t>
         </is>
       </c>
     </row>
@@ -1636,12 +1636,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>D836FA75F0682B4C393418231AEFCA97169D551E</t>
+          <t>d9e94f076d175ace80f211ea298fa46e</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'd9e94f076d175ace80f211ea298fa46e' combination.</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>7BD85FEE9A79D2AAD47AC9F299B12FE0</t>
+          <t>5cc861346ab9f1980a919f70671894e8</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '7bd85fee9a79d2aad47ac9f299b12fe0' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '5cc861346ab9f1980a919f70671894e8' combination.</t>
         </is>
       </c>
     </row>
@@ -1686,12 +1686,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>140.82.49.12</t>
+          <t>http://hotelamerpalace.com/Fox-C404/LEPqPJpt4Gbr8BHAn/</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '140.82.49.12' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>a66c2a67287a0781e18305076359a30a9bd5b23683feecc5ff7e82a01383e2b8</t>
+          <t>9bda03babb0f2c6aa9861eca95b33af06a650e2851cce4edcc1fc3abd8e7c2a1</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'a66c2a67287a0781e18305076359a30a9bd5b23683feecc5ff7e82a01383e2b8' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '9bda03babb0f2c6aa9861eca95b33af06a650e2851cce4edcc1fc3abd8e7c2a1' combination.</t>
         </is>
       </c>
     </row>
@@ -1736,12 +1736,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>acfd5ff345a01a7107b63100a930c2a63fbd50aac738c6e8207eeb7c3cfcdcb5</t>
+          <t>http://unifiedpharma.com/wp-content/5arxM/</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'acfd5ff345a01a7107b63100a930c2a63fbd50aac738c6e8207eeb7c3cfcdcb5' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>F615ED88710B54131443555EE7F7EA97</t>
+          <t>151c6f04aeff0e00c54929f25328f6f7</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'f615ed88710b54131443555ee7f7ea97' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '151c6f04aeff0e00c54929f25328f6f7' combination.</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>684d87809604a15d9f49bd5dee29fb6e</t>
+          <t>405cb8b1e55bb2a50f2ef3e7c2b28496</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '684d87809604a15d9f49bd5dee29fb6e' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '405cb8b1e55bb2a50f2ef3e7c2b28496' combination.</t>
         </is>
       </c>
     </row>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ec471e89fa74c32dc6e0fbccbdaa9e5dd42c0696</t>
+          <t>d66c9164299ab76066cd3d883b2ad4bfe0c8f4c6</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>f08c8e6bf954497390c5cc140745b579</t>
+          <t>4b211f3c2cc9a1605db36043cb2b2e0e</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1851,7 +1851,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'f08c8e6bf954497390c5cc140745b579' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '4b211f3c2cc9a1605db36043cb2b2e0e' combination.</t>
         </is>
       </c>
     </row>
@@ -1861,12 +1861,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>AA5C39DE77F15A91ED580E7A0F132EB14C970235</t>
+          <t>eed7357ab8d2fe31ea3dbcf3f9b7ec74</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'eed7357ab8d2fe31ea3dbcf3f9b7ec74' combination.</t>
         </is>
       </c>
     </row>
@@ -1886,12 +1886,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>B6ED9B2819915C2B57D4C58E37C08BA4</t>
+          <t>1d772f707ce74473996c377477ad718bba495fe7cd022d5b802aaf32c853f115</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'b6ed9b2819915c2b57d4c58e37c08ba4' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '1d772f707ce74473996c377477ad718bba495fe7cd022d5b802aaf32c853f115' combination.</t>
         </is>
       </c>
     </row>
@@ -1911,12 +1911,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>185.250.148.74</t>
+          <t>3215decffc40b3257ebeb9b6e5c81c45e298a020f33ef90c9418c153c6071b36</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '185.250.148.74' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '3215decffc40b3257ebeb9b6e5c81c45e298a020f33ef90c9418c153c6071b36' combination.</t>
         </is>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>46.105.81.76</t>
+          <t>95.181.152.184</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '46.105.81.76' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '95.181.152.184' combination.</t>
         </is>
       </c>
     </row>
@@ -1961,12 +1961,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>86CBF834C23A31B6791E47B7C34B515555FDDAF4</t>
+          <t>7c76ca5eb757df4362fabb8cff1deaa92ebc31a17786c89bde55bc53ada43864</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '7c76ca5eb757df4362fabb8cff1deaa92ebc31a17786c89bde55bc53ada43864' combination.</t>
         </is>
       </c>
     </row>
@@ -1986,12 +1986,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Domain</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>privacytoolzforyou7000.top</t>
+          <t>9344afc63753cd5e2ee0ff9aed43dc56</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'domain' and value: 'privacytoolzforyou7000.top' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '9344afc63753cd5e2ee0ff9aed43dc56' combination.</t>
         </is>
       </c>
     </row>
@@ -2011,12 +2011,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>e6c1b0f47b9240a8ce2aa9705c930c5dd5b98c046687158116637da10cafc493</t>
+          <t>f8c9cb79423380b18cbd03d9986766c95f9fd392</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'e6c1b0f47b9240a8ce2aa9705c930c5dd5b98c046687158116637da10cafc493' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>4554DC95F99D6682595812B677FB131A7E7C51A71DAF461A57A57A0D903BB3FA</t>
+          <t>0f0cabb24d8cc93e5aed340cfc492c4008509f1e84311d61721a4375260a0911</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '4554dc95f99d6682595812b677fb131a7e7c51a71daf461a57a57a0d903bb3fa' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '0f0cabb24d8cc93e5aed340cfc492c4008509f1e84311d61721a4375260a0911' combination.</t>
         </is>
       </c>
     </row>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>54753CA6879AB9F1D06264147CDF466B</t>
+          <t>4d2da36174633565f3dd5ed6dc5033c4</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '54753ca6879ab9f1d06264147cdf466b' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '4d2da36174633565f3dd5ed6dc5033c4' combination.</t>
         </is>
       </c>
     </row>
@@ -2086,12 +2086,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>E0FAFE1B4EB787444ED457DBF05895A4</t>
+          <t>91f8592c7e8a3091273f0ccbfe34b2586c5998f7de63130050cb8ed36b4eec3e</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'e0fafe1b4eb787444ed457dbf05895a4' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '91f8592c7e8a3091273f0ccbfe34b2586c5998f7de63130050cb8ed36b4eec3e' combination.</t>
         </is>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2B32F3A1BCFCE9F6DB00CF4C0FEEB291F6514AEE</t>
+          <t>d3f4efc5d5343a54fabb94507d1197cb7e088a93</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>105.198.236.99</t>
+          <t>296c51eb03e70808304b5f0e050f4f94</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '105.198.236.99' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '296c51eb03e70808304b5f0e050f4f94' combination.</t>
         </is>
       </c>
     </row>
@@ -2161,12 +2161,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>16B5B1494E211B74E97D9F35FF5A994F70411F2E</t>
+          <t>c010d1326689b95a3d8106f75003427c</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'c010d1326689b95a3d8106f75003427c' combination.</t>
         </is>
       </c>
     </row>
@@ -2186,12 +2186,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>ipv4</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>929A591331BDC1972357059D451A651D575166F676EA51DAAEB358AA2A1064B7</t>
+          <t>91.240.118.168</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '929a591331bdc1972357059d451a651d575166f676ea51daaeb358aa2a1064b7' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '91.240.118.168' combination.</t>
         </is>
       </c>
     </row>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2F4085CB6A0B2DD4422F59894DCA5CF881EB8CCF</t>
+          <t>f2d41df1d55178b5f7de0512912159f2663296cd</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2236,12 +2236,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>24.229.150.54</t>
+          <t>ad29212716d0b074d976ad7e33b8f35f</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '24.229.150.54' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'ad29212716d0b074d976ad7e33b8f35f' combination.</t>
         </is>
       </c>
     </row>
@@ -2261,12 +2261,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>17BB787FEE1B83990F47DDAEAA81EFC26F04457D</t>
+          <t>a9cf6dce244ad9afd8ca92820b9c11b9</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'a9cf6dce244ad9afd8ca92820b9c11b9' combination.</t>
         </is>
       </c>
     </row>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>88834D17D2CDCE884A73E38638A4E0DD</t>
+          <t>dfcb2501be0a877c79c6abfb9cf17397</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '88834d17d2cdce884a73e38638a4e0dd' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'dfcb2501be0a877c79c6abfb9cf17397' combination.</t>
         </is>
       </c>
     </row>
@@ -2311,12 +2311,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>88319E075EE9D7092A11A1E0237EE16C</t>
+          <t>1b23b966249a1da92300f3b857b40da8d8cd549a</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '88319e075ee9d7092a11a1e0237ee16c' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2336,12 +2336,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>FCC49C9BE5591F241FFD98DB0752CB9E20A97E881969537FBA5C513ADBD72814</t>
+          <t>695e343b81a7b0208cbae33e11f7044c</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'fcc49c9be5591f241ffd98db0752cb9e20a97e881969537fba5c513adbd72814' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '695e343b81a7b0208cbae33e11f7044c' combination.</t>
         </is>
       </c>
     </row>
@@ -2361,12 +2361,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>56839287637B98F12187E61EA5626E21</t>
+          <t>956876902f17d6fabbcdbfeb38428a2b50045270</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '56839287637b98f12187e61ea5626e21' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2386,12 +2386,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>173.25.166.81</t>
+          <t>e0e4251386cdf8fe716d0779c3868e00d4ecc879</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '173.25.166.81' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2411,12 +2411,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>89.101.97.139</t>
+          <t>58f01d40edb624cecd22aab1ff139da9</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '89.101.97.139' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '58f01d40edb624cecd22aab1ff139da9' combination.</t>
         </is>
       </c>
     </row>
@@ -2436,12 +2436,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>196.218.227.241</t>
+          <t>6d55f25222831cce73fd9a64a8e5a63b002522dc2637bd2704f77168c7c02d88</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '196.218.227.241' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '6d55f25222831cce73fd9a64a8e5a63b002522dc2637bd2704f77168c7c02d88' combination.</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>5DD964C8D9025224EB658F96034BABEA</t>
+          <t>c13bf39e2f8bf49c9754de7fb1396a33</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '5dd964c8d9025224eb658f96034babea' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'c13bf39e2f8bf49c9754de7fb1396a33' combination.</t>
         </is>
       </c>
     </row>
@@ -2486,12 +2486,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Domain</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>privacy-toolz-for-you-403.top</t>
+          <t>618ea7b0e2a26f3c6db0a8664c63fc6f</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'domain' and value: 'privacy-toolz-for-you-403.top' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '618ea7b0e2a26f3c6db0a8664c63fc6f' combination.</t>
         </is>
       </c>
     </row>
@@ -2511,12 +2511,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>6ABBD89E6AB5E1B63C38A8F78271A97D19BAFFF4959EA9D5BD5DA3B185EB61E6</t>
+          <t>a5c353d06ea4f59570429b5a7a2017204adb40a1</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '6abbd89e6ab5e1b63c38a8f78271a97d19bafff4959ea9d5bd5da3b185eb61e6' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>AD413CD422C1A0355163618683E936A0</t>
+          <t>52b8ae74406e2f52fd81c8458647acd8</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: 'ad413cd422c1a0355163618683e936a0' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '52b8ae74406e2f52fd81c8458647acd8' combination.</t>
         </is>
       </c>
     </row>
@@ -2561,12 +2561,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA-1</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>43660D21BFA1431E0EE3426CD12DDF38</t>
+          <t>a6068f6f7acdff5de9ce992889a69e61033a1524</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '43660d21bfa1431e0ee3426cd12ddf38' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2586,12 +2586,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Domain</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>privacytoolzforyou-6000.top</t>
+          <t>a77899602387665cddb6a0f021184a2b</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'domain' and value: 'privacytoolzforyou-6000.top' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'a77899602387665cddb6a0f021184a2b' combination.</t>
         </is>
       </c>
     </row>
@@ -2611,12 +2611,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>68.204.7.158</t>
+          <t>48c2f53f1eeb669fadb3eec46f7f3d4572e819c7bb2d39f22d22713a30cc1846</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '68.204.7.158' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '48c2f53f1eeb669fadb3eec46f7f3d4572e819c7bb2d39f22d22713a30cc1846' combination.</t>
         </is>
       </c>
     </row>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>56839287637B98F12187E61EA5626E21</t>
+          <t>0c524b45d37f4fe2c2ac378478516853</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '56839287637b98f12187e61ea5626e21' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '0c524b45d37f4fe2c2ac378478516853' combination.</t>
         </is>
       </c>
     </row>
@@ -2661,12 +2661,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>9D12105B2E0055A86A3EA9F284718E2CE60D3E74</t>
+          <t>2de72908e0a1ef97e4e06d8b1ba3dc0d76f580cdf36f96b5c919bea770b2805f</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '2de72908e0a1ef97e4e06d8b1ba3dc0d76f580cdf36f96b5c919bea770b2805f' combination.</t>
         </is>
       </c>
     </row>
@@ -2686,12 +2686,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>70A49561F39BB362A2EF79DB15E326812912C17D6E6EB38EF40343A95409A19A</t>
+          <t>11e35160fc4efabd0a3bd7a7c6afc91b</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '70a49561f39bb362a2ef79db15e326812912c17d6e6eb38ef40343a95409a19a' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '11e35160fc4efabd0a3bd7a7c6afc91b' combination.</t>
         </is>
       </c>
     </row>
@@ -2711,12 +2711,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>188776C2BDD001D6A57B1CFC7E156DD3</t>
+          <t>d742a33692a77f5caef5ea175957c98b56c2dc255144784ad3bade0a0d50d088</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '188776c2bdd001d6a57b1cfc7e156dd3' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: 'd742a33692a77f5caef5ea175957c98b56c2dc255144784ad3bade0a0d50d088' combination.</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>7332A59679C7732855D11DFF20061A76</t>
+          <t>cd7034692d8f29f9146deb3641de7986</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2751,7 +2751,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '7332a59679c7732855d11dff20061a76' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'cd7034692d8f29f9146deb3641de7986' combination.</t>
         </is>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>136.232.34.70</t>
+          <t>185.112.83.22</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '136.232.34.70' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '185.112.83.22' combination.</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>AAE0553B761E8BB3E58902A46CD98EE68310252734D1F8D9FD3B862AAB8ED5C9</t>
+          <t>9f22626232934970e4851467b7b746578f0f149984cd0e4e1a156b391727fac9</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'aae0553b761e8bb3e58902a46cd98ee68310252734d1f8d9fd3b862aab8ed5c9' combination.</t>
+          <t>severity: The 'severity' field must contain a valid severity. Allowed values: [informational low medium high critical].</t>
         </is>
       </c>
     </row>
@@ -2811,12 +2811,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>95.77.223.148</t>
+          <t>d2a15e76a4bfa7eb007a07fc8738edfb</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '95.77.223.148' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'd2a15e76a4bfa7eb007a07fc8738edfb' combination.</t>
         </is>
       </c>
     </row>
@@ -2836,12 +2836,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>72.252.201.69</t>
+          <t>e2eb5b57a8765856be897b4f6dadca18</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '72.252.201.69' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'e2eb5b57a8765856be897b4f6dadca18' combination.</t>
         </is>
       </c>
     </row>
@@ -2861,12 +2861,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>79A90C8BC6FD6179CB91D2EA2666124B</t>
+          <t>https://connecticutsfinestmovers.com/Fox-C/mVwOqxT17gVWaE8E/</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '79a90c8bc6fd6179cb91d2ea2666124b' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -2886,12 +2886,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>5FCA07DFC68A13B3707636440D5C416E56149357</t>
+          <t>5bd4987db7e6946bf2ca3f73e17d6f75e2d8217df63b2f7763ea9a6ebcaf9fed</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '5bd4987db7e6946bf2ca3f73e17d6f75e2d8217df63b2f7763ea9a6ebcaf9fed' combination.</t>
         </is>
       </c>
     </row>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2615BD2173DAC44A6AD14702F3C93E67</t>
+          <t>df7befc8cdc3c5434ef27cc669fb1e4b</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '2615bd2173dac44a6ad14702f3c93e67' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'df7befc8cdc3c5434ef27cc669fb1e4b' combination.</t>
         </is>
       </c>
     </row>
@@ -2936,12 +2936,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>EEF15F6416F756693CBFBFD8650CCB665771B54B4CC31CB09AEEA0D13EC640CF</t>
+          <t>a4bd130d0ea5e3ab8060464620e742a8</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'eef15f6416f756693cbfbfd8650ccb665771b54b4cc31cb09aeea0d13ec640cf' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'a4bd130d0ea5e3ab8060464620e742a8' combination.</t>
         </is>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>5D3B7E0C05E65AA0DFC8B5E48142D782352E36BE</t>
+          <t>6590b5b2578da2374b846ae15a0307fa3ce33f33</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2986,12 +2986,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1411250EB56C55E274FBCF0741BBD3B5C917167D153779C7D8041AB2627EF95F</t>
+          <t>04256e521917757926de32e6b7405cc7</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '1411250eb56c55e274fbcf0741bbd3b5c917167d153779c7d8041ab2627ef95f' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '04256e521917757926de32e6b7405cc7' combination.</t>
         </is>
       </c>
     </row>
@@ -3011,12 +3011,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>5ADBE8D0375D6531F1A523085F4DF4151AD1BD7AE539692E2CAA3D0D73301293</t>
+          <t>http://icfacn.com/runtime/n7qA2YStudp/</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '5adbe8d0375d6531f1a523085f4df4151ad1bd7ae539692e2caa3d0d73301293' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>21c2867e81b6f78c2fecba181c8bc7a51fc82a99</t>
+          <t>ee1fa399ace734c33b77c62b6fb010219580448f</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>af41c3193257d3cbd07e5a9e1cb6fd6011101a40</t>
+          <t>c90f32fd0fd4eefe752b7b3f7ebfbc7bd9092b16</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3086,12 +3086,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>304D8E812A8D988E21AF8A865D8DD577DC6F3134</t>
+          <t>e46bfbdf1031ea5a383040d0aa598d45</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'e46bfbdf1031ea5a383040d0aa598d45' combination.</t>
         </is>
       </c>
     </row>
@@ -3111,12 +3111,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>5bd8befa1fad2b4b7d2d67a52625e083799354e5</t>
+          <t>40e1656f65b472375735feef8d9d1197</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: '40e1656f65b472375735feef8d9d1197' combination.</t>
         </is>
       </c>
     </row>
@@ -3136,12 +3136,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>ipv4</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>BF7B5F72B2055CFC8DA01BB48CF5AE8E45E523860E0B23A65B9F14DBDBB7F4EE</t>
+          <t>185.206.212.165</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'bf7b5f72b2055cfc8da01bb48cf5ae8e45e523860e0b23a65b9f14dbdbb7f4ee' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '185.206.212.165' combination.</t>
         </is>
       </c>
     </row>
@@ -3161,12 +3161,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>SHA256</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>24.139.72.117</t>
+          <t>2ced68e4425d31cca494557c29a76dfc3081f594ff01549e41d2f8a08923ef61</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '24.139.72.117' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '2ced68e4425d31cca494557c29a76dfc3081f594ff01549e41d2f8a08923ef61' combination.</t>
         </is>
       </c>
     </row>
@@ -3186,12 +3186,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>47.22.148.6</t>
+          <t>659b77f88288b4874b5abe41ed36380d</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '47.22.148.6' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '659b77f88288b4874b5abe41ed36380d' combination.</t>
         </is>
       </c>
     </row>
@@ -3211,12 +3211,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>495388cc2be9ad2ac6555dcc1711a9e84a43dd373e1f27629a2e335c43abcfbb</t>
+          <t>https://krezol-group.com:443/images/PmLGLKYeCBs5d/</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '495388cc2be9ad2ac6555dcc1711a9e84a43dd373e1f27629a2e335c43abcfbb' combination.</t>
+          <t>Type is not valid</t>
         </is>
       </c>
     </row>
@@ -3236,12 +3236,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>ipv4</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>120.150.218.241</t>
+          <t>ae6fbc60ba9c0f3a0fef72aeffcd3dc7</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '120.150.218.241' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'ae6fbc60ba9c0f3a0fef72aeffcd3dc7' combination.</t>
         </is>
       </c>
     </row>
@@ -3261,12 +3261,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>46c6f2719d05edb434a831e82bcaf1827cad665d</t>
+          <t>http://ledcaopingdeng.com/wp-includes/Qq39yj7fpvk/</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3286,12 +3286,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>65202b343ccc9753d39f3cb2ff1436ac17a9fb88a6e296ef166e64e6e3b7daea</t>
+          <t>8dfa48e56fc3a6a2272771e708cdb4d2</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '65202b343ccc9753d39f3cb2ff1436ac17a9fb88a6e296ef166e64e6e3b7daea' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '8dfa48e56fc3a6a2272771e708cdb4d2' combination.</t>
         </is>
       </c>
     </row>
@@ -3311,12 +3311,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>c8d0aec9e1e1d2fec33726b24ea7675484127bef</t>
+          <t>b8e24e6436f6bed17757d011780e87b9</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: 'b8e24e6436f6bed17757d011780e87b9' combination.</t>
         </is>
       </c>
     </row>
@@ -3336,12 +3336,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>24e955ba66911deab068c74fa9956a259ad041ba</t>
+          <t>http://autodiscover.karlamejia.com/wp-admin/hcdnVlRIiwvTVrJjJEE/</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3361,12 +3361,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>03E96FC686CC15A0BB26186ECB4FE63E6B841C4B</t>
+          <t>44baa1595e5294ad4464a2cd567b2b6e</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: '44baa1595e5294ad4464a2cd567b2b6e' combination.</t>
         </is>
       </c>
     </row>
@@ -3391,7 +3391,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>173.21.10.71</t>
+          <t>65.21.105.85</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '173.21.10.71' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '65.21.105.85' combination.</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>71d721dfbd6c375c327a8470f0664b53cfce5f50303145bbd5f837ffd8b48a6a</t>
+          <t>095c223b94656622c81cb9386aefa59e168756c3e200457e98c00b609e0bb170</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3426,7 +3426,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '71d721dfbd6c375c327a8470f0664b53cfce5f50303145bbd5f837ffd8b48a6a' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: '095c223b94656622c81cb9386aefa59e168756c3e200457e98c00b609e0bb170' combination.</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>E510566244A899D6A427C1648E680A2310C170A5F25AFF53B15D8DE52CA11767</t>
+          <t>dcaaef3509bc75155789058d79f025f14166386cec833c2c154ca34cfea26c52</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'e510566244a899d6a427c1648e680a2310c170a5f25aff53b15d8de52ca11767' combination.</t>
+          <t>Warning: Duplicate type: 'sha256' and value: 'dcaaef3509bc75155789058d79f025f14166386cec833c2c154ca34cfea26c52' combination.</t>
         </is>
       </c>
     </row>
@@ -3461,12 +3461,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>17BB787FEE1B83990F47DDAEAA81EFC26F04457D</t>
+          <t>51f2cf541f004d3c1fa8b0f94c89914a</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: '51f2cf541f004d3c1fa8b0f94c89914a' combination.</t>
         </is>
       </c>
     </row>
@@ -3486,12 +3486,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>SHA256</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>A0538746CE241A518E3A056789EA60671F626613DD92F3CAA5A95E92E65357B3</t>
+          <t>8320d9ec2eab7f5ff49186b2e630a15f</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'a0538746ce241a518e3a056789ea60671f626613dd92f3caa5a95e92e65357b3' combination.</t>
+          <t>Warning: Duplicate type: 'md5' and value: '8320d9ec2eab7f5ff49186b2e630a15f' combination.</t>
         </is>
       </c>
     </row>
@@ -3511,12 +3511,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>SHA-1</t>
+          <t>MD5</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>F94D5BF14DEE6A6E8DB957D49C259082DD82350B</t>
+          <t>1473c91e9c0588f92928bed0ebf5e0f4</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3526,7 +3526,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Type is not valid</t>
+          <t>Warning: Duplicate type: 'md5' and value: '1473c91e9c0588f92928bed0ebf5e0f4' combination.</t>
         </is>
       </c>
     </row>
@@ -3536,12 +3536,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>MD5</t>
+          <t>ipv4</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>353A21B3835AC7C17A82AF79302D23CC</t>
+          <t>91.240.118.168</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3551,7 +3551,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'md5' and value: '353a21b3835ac7c17a82af79302d23cc' combination.</t>
+          <t>Warning: Duplicate type: 'ipv4' and value: '91.240.118.168' combination.</t>
         </is>
       </c>
     </row>
@@ -3561,12 +3561,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Domain</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>privacy-tools-for-you-777.com</t>
+          <t>http://artanddesign.one/wp-content/uploads/A2cZL7/</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3576,257 +3576,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Warning: Duplicate type: 'domain' and value: 'privacy-tools-for-you-777.com' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>MD5</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>2A8CF6154E6A129FFD07A501BBC0B098</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'md5' and value: '2a8cf6154e6a129ffd07a501bbc0b098' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>ipv4</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>45.46.53.140</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '45.46.53.140' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>127</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>SHA256</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>850ba59403825d4feebbff0112c448143ebe8b872040e7383f201b9b101ae4bc</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'sha256' and value: '850ba59403825d4feebbff0112c448143ebe8b872040e7383f201b9b101ae4bc' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>MD5</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>0b16c4d406c5b85aa372f6d14fe1ed28</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'md5' and value: '0b16c4d406c5b85aa372f6d14fe1ed28' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>SHA-1</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>B5B264D00A7D6D6B3DD4965DBE2BD00E0823BA6C</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
           <t>Type is not valid</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>SHA-1</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>A295F15F38F8D4E83B5DB8F51ADDAE2D2DF328DD</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>Type is not valid</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>MD5</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>000DF43B256CDC27BB22870919BB1DFA</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'md5' and value: '000df43b256cdc27bb22870919bb1dfa' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="n">
-        <v>132</v>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>MD5</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>09a2ab61f1a4bf561025dd98473c4309</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'md5' and value: '09a2ab61f1a4bf561025dd98473c4309' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>133</v>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>SHA256</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>F9246BE51464E71FF6B37975CD44359E8576F2BF03CB4028E536D7CFDE3508FC</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'sha256' and value: 'f9246be51464e71ff6b37975cd44359e8576f2bf03cb4028e536d7cfde3508fc' combination.</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>134</v>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>ipv4</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>185.7.214.7</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Warning: Duplicate type: 'ipv4' and value: '185.7.214.7' combination.</t>
         </is>
       </c>
     </row>

</xml_diff>